<commit_message>
Raw data transformation fix and cleaning of previous results
The hotfixes for the real growth rate in raw data transformation are included´that we programmed in the evening of 7th March with Zexi Sun.
</commit_message>
<xml_diff>
--- a/MMB_Estimation/RawDataTransformation/usrawdata/SPFRGDP.xlsx
+++ b/MMB_Estimation/RawDataTransformation/usrawdata/SPFRGDP.xlsx
@@ -100,21 +100,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -425,54 +419,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L201"/>
+  <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202:XFD238"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection sqref="A1:L202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.100000000000001" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7669,31 +7663,31 @@
         <v>16442.3</v>
       </c>
       <c r="D191" s="5">
-        <v>16524.91</v>
+        <v>16524.912700000001</v>
       </c>
       <c r="E191" s="5">
-        <v>16623.64</v>
+        <v>16623.6387</v>
       </c>
       <c r="F191" s="5">
-        <v>16728.349999999999</v>
+        <v>16728.345099999999</v>
       </c>
       <c r="G191" s="5">
-        <v>16833.48</v>
+        <v>16833.479800000001</v>
       </c>
       <c r="H191" s="5">
-        <v>16928.8</v>
+        <v>16928.802299999999</v>
       </c>
       <c r="I191" s="5">
-        <v>16679.66</v>
+        <v>16679.6607</v>
       </c>
       <c r="J191" s="5">
-        <v>17080.310000000001</v>
+        <v>17080.314200000001</v>
       </c>
       <c r="K191" s="5">
-        <v>17526.04</v>
+        <v>17526.044300000001</v>
       </c>
       <c r="L191" s="5">
-        <v>17934.47</v>
+        <v>17934.467199999999</v>
       </c>
     </row>
     <row r="192" spans="1:12" ht="15" customHeight="1">
@@ -7704,34 +7698,34 @@
         <v>2</v>
       </c>
       <c r="C192" s="5">
-        <v>16492.7</v>
+        <v>16492.7012</v>
       </c>
       <c r="D192" s="5">
-        <v>16581.189999999999</v>
+        <v>16581.186699999998</v>
       </c>
       <c r="E192" s="5">
-        <v>16677.64</v>
+        <v>16677.635699999999</v>
       </c>
       <c r="F192" s="5">
-        <v>16780.830000000002</v>
+        <v>16780.831900000001</v>
       </c>
       <c r="G192" s="5">
-        <v>16872.27</v>
+        <v>16872.272400000002</v>
       </c>
       <c r="H192" s="5">
-        <v>16973.34</v>
+        <v>16973.336599999999</v>
       </c>
       <c r="I192" s="5">
-        <v>16633.5</v>
+        <v>16633.5039</v>
       </c>
       <c r="J192" s="5">
-        <v>17025.740000000002</v>
+        <v>17025.741699999999</v>
       </c>
       <c r="K192" s="5">
-        <v>17427.77</v>
+        <v>17427.771700000001</v>
       </c>
       <c r="L192" s="5">
-        <v>17829.29</v>
+        <v>17829.293699999998</v>
       </c>
     </row>
     <row r="193" spans="1:12" ht="15" customHeight="1">
@@ -7742,34 +7736,34 @@
         <v>3</v>
       </c>
       <c r="C193" s="5">
-        <v>16575.099999999999</v>
+        <v>16575.0995</v>
       </c>
       <c r="D193" s="5">
-        <v>16690.03</v>
+        <v>16690.032200000001</v>
       </c>
       <c r="E193" s="5">
-        <v>16787.439999999999</v>
+        <v>16787.4434</v>
       </c>
       <c r="F193" s="5">
-        <v>16875.759999999998</v>
+        <v>16875.761600000002</v>
       </c>
       <c r="G193" s="5">
-        <v>16970.75</v>
+        <v>16970.751700000001</v>
       </c>
       <c r="H193" s="5">
-        <v>17066.22</v>
+        <v>17066.220099999999</v>
       </c>
       <c r="I193" s="5">
-        <v>16645.84</v>
+        <v>16645.838</v>
       </c>
       <c r="J193" s="5">
-        <v>17016.740000000002</v>
+        <v>17016.7372</v>
       </c>
       <c r="K193" s="5">
-        <v>17409.16</v>
+        <v>17409.158100000001</v>
       </c>
       <c r="L193" s="5">
-        <v>17804.02</v>
+        <v>17804.0249</v>
       </c>
     </row>
     <row r="194" spans="1:12" ht="15" customHeight="1">
@@ -7780,34 +7774,34 @@
         <v>4</v>
       </c>
       <c r="C194" s="5">
-        <v>16701.57</v>
+        <v>16701.572499999998</v>
       </c>
       <c r="D194" s="5">
-        <v>16792.349999999999</v>
+        <v>16792.348099999999</v>
       </c>
       <c r="E194" s="5">
-        <v>16884.55</v>
+        <v>16884.5497</v>
       </c>
       <c r="F194" s="5">
-        <v>16984.95</v>
+        <v>16984.9532</v>
       </c>
       <c r="G194" s="5">
-        <v>17081.599999999999</v>
+        <v>17081.599900000001</v>
       </c>
       <c r="H194" s="5">
-        <v>17176.599999999999</v>
+        <v>17176.599699999999</v>
       </c>
       <c r="I194" s="5">
-        <v>16650.57</v>
+        <v>16650.5717</v>
       </c>
       <c r="J194" s="5">
-        <v>17030.78</v>
+        <v>17030.782200000001</v>
       </c>
       <c r="K194" s="5">
-        <v>17405.86</v>
+        <v>17405.860700000001</v>
       </c>
       <c r="L194" s="5">
-        <v>17821.13</v>
+        <v>17821.129099999998</v>
       </c>
     </row>
     <row r="195" spans="1:12" ht="15" customHeight="1">
@@ -7821,31 +7815,31 @@
         <v>16804.8</v>
       </c>
       <c r="D195" s="5">
-        <v>16901.27</v>
+        <v>16901.2729</v>
       </c>
       <c r="E195" s="5">
-        <v>16998.34</v>
+        <v>16998.335299999999</v>
       </c>
       <c r="F195" s="5">
-        <v>17099.509999999998</v>
+        <v>17099.513800000001</v>
       </c>
       <c r="G195" s="5">
-        <v>17198.91</v>
+        <v>17198.906299999999</v>
       </c>
       <c r="H195" s="5">
-        <v>17305.72</v>
+        <v>17305.7156</v>
       </c>
       <c r="I195" s="5">
-        <v>17050.560000000001</v>
+        <v>17050.561000000002</v>
       </c>
       <c r="J195" s="5">
-        <v>17467.330000000002</v>
+        <v>17467.331099999999</v>
       </c>
       <c r="K195" s="5">
-        <v>17894.29</v>
+        <v>17894.293600000001</v>
       </c>
       <c r="L195" s="5">
-        <v>18286.310000000001</v>
+        <v>18286.305799999998</v>
       </c>
     </row>
     <row r="196" spans="1:12" ht="15" customHeight="1">
@@ -7859,31 +7853,31 @@
         <v>16842.400000000001</v>
       </c>
       <c r="D196" s="5">
-        <v>16972.580000000002</v>
+        <v>16972.581999999999</v>
       </c>
       <c r="E196" s="5">
-        <v>17081.490000000002</v>
+        <v>17081.491399999999</v>
       </c>
       <c r="F196" s="5">
-        <v>17184.91</v>
+        <v>17184.912400000001</v>
       </c>
       <c r="G196" s="5">
-        <v>17284.64</v>
+        <v>17284.638200000001</v>
       </c>
       <c r="H196" s="5">
-        <v>17398.8</v>
+        <v>17398.7997</v>
       </c>
       <c r="I196" s="5">
-        <v>17020.23</v>
+        <v>17020.225200000001</v>
       </c>
       <c r="J196" s="5">
-        <v>17449.72</v>
+        <v>17449.720700000002</v>
       </c>
       <c r="K196" s="5">
-        <v>17857.47</v>
+        <v>17857.466499999999</v>
       </c>
       <c r="L196" s="5">
-        <v>18266.57</v>
+        <v>18266.565500000001</v>
       </c>
     </row>
     <row r="197" spans="1:12" ht="15" customHeight="1">
@@ -7894,34 +7888,34 @@
         <v>3</v>
       </c>
       <c r="C197" s="5">
-        <v>17010.7</v>
+        <v>17010.699499999999</v>
       </c>
       <c r="D197" s="5">
-        <v>17125.02</v>
+        <v>17125.024000000001</v>
       </c>
       <c r="E197" s="5">
-        <v>17226.54</v>
+        <v>17226.5406</v>
       </c>
       <c r="F197" s="5">
-        <v>17324.02</v>
+        <v>17324.019100000001</v>
       </c>
       <c r="G197" s="5">
-        <v>17428.13</v>
+        <v>17428.131700000002</v>
       </c>
       <c r="H197" s="5">
-        <v>17536.689999999999</v>
+        <v>17536.6898</v>
       </c>
       <c r="I197" s="5">
-        <v>17066.509999999998</v>
+        <v>17066.514800000001</v>
       </c>
       <c r="J197" s="5">
-        <v>17484.57</v>
+        <v>17484.573899999999</v>
       </c>
       <c r="K197" s="5">
-        <v>17886.009999999998</v>
+        <v>17886.011999999999</v>
       </c>
       <c r="L197" s="5">
-        <v>18267.22</v>
+        <v>18267.217700000001</v>
       </c>
     </row>
     <row r="198" spans="1:12" ht="15" customHeight="1">
@@ -7935,31 +7929,31 @@
         <v>17156.900000000001</v>
       </c>
       <c r="D198" s="5">
-        <v>17270.16</v>
+        <v>17270.1639</v>
       </c>
       <c r="E198" s="5">
-        <v>17371.23</v>
+        <v>17371.229299999999</v>
       </c>
       <c r="F198" s="5">
-        <v>17479.169999999998</v>
+        <v>17479.167700000002</v>
       </c>
       <c r="G198" s="5">
-        <v>17582.88</v>
+        <v>17582.883699999998</v>
       </c>
       <c r="H198" s="5">
-        <v>17684.02</v>
+        <v>17684.021700000001</v>
       </c>
       <c r="I198" s="5">
-        <v>17090.240000000002</v>
+        <v>17090.236199999999</v>
       </c>
       <c r="J198" s="5">
-        <v>17529.78</v>
+        <v>17529.7775</v>
       </c>
       <c r="K198" s="5">
-        <v>17929.419999999998</v>
+        <v>17929.4247</v>
       </c>
       <c r="L198" s="5">
-        <v>18276.88</v>
+        <v>18276.883099999999</v>
       </c>
     </row>
     <row r="199" spans="1:12">
@@ -7973,31 +7967,31 @@
         <v>17272.5</v>
       </c>
       <c r="D199" s="5">
-        <v>17403.2</v>
+        <v>17403.196100000001</v>
       </c>
       <c r="E199" s="5">
-        <v>17524.990000000002</v>
+        <v>17524.991399999999</v>
       </c>
       <c r="F199" s="5">
-        <v>17642.37</v>
+        <v>17642.369900000002</v>
       </c>
       <c r="G199" s="5">
-        <v>17753.16</v>
+        <v>17753.164799999999</v>
       </c>
       <c r="H199" s="5">
-        <v>17865.490000000002</v>
+        <v>17865.490399999999</v>
       </c>
       <c r="I199" s="5">
-        <v>17580.88</v>
+        <v>17580.880700000002</v>
       </c>
       <c r="J199" s="5">
-        <v>18014.400000000001</v>
+        <v>18014.400300000001</v>
       </c>
       <c r="K199" s="5">
-        <v>18382.36</v>
+        <v>18382.356400000001</v>
       </c>
       <c r="L199" s="5">
-        <v>18733.89</v>
+        <v>18733.890200000002</v>
       </c>
     </row>
     <row r="200" spans="1:12">
@@ -8011,69 +8005,107 @@
         <v>17385.8</v>
       </c>
       <c r="D200" s="5">
-        <v>17522.04</v>
+        <v>17522.043900000001</v>
       </c>
       <c r="E200" s="5">
-        <v>17649.25</v>
+        <v>17649.254300000001</v>
       </c>
       <c r="F200" s="5">
-        <v>17767.349999999999</v>
+        <v>17767.346699999998</v>
       </c>
       <c r="G200" s="5">
-        <v>17880.71</v>
+        <v>17880.714</v>
       </c>
       <c r="H200" s="5">
-        <v>17994.830000000002</v>
+        <v>17994.831900000001</v>
       </c>
       <c r="I200" s="5">
-        <v>17582.71</v>
+        <v>17582.714599999999</v>
       </c>
       <c r="J200" s="5">
-        <v>18047.2</v>
+        <v>18047.195899999999</v>
       </c>
       <c r="K200" s="5">
-        <v>18420.09</v>
+        <v>18420.091499999999</v>
       </c>
       <c r="L200" s="5">
-        <v>18818.57</v>
+        <v>18818.5694</v>
       </c>
     </row>
     <row r="201" spans="1:12">
       <c r="A201" s="4">
         <v>2018</v>
       </c>
-      <c r="B201" s="6">
+      <c r="B201" s="4">
         <v>3</v>
       </c>
-      <c r="C201" s="7">
+      <c r="C201" s="5">
         <v>18507.2</v>
       </c>
-      <c r="D201" s="7">
+      <c r="D201" s="5">
         <v>18645.916700000002</v>
       </c>
-      <c r="E201" s="7">
+      <c r="E201" s="5">
         <v>18776.3331</v>
       </c>
-      <c r="F201" s="7">
+      <c r="F201" s="5">
         <v>18892.792300000001</v>
       </c>
-      <c r="G201" s="7">
+      <c r="G201" s="5">
         <v>19011.684000000001</v>
       </c>
-      <c r="H201" s="7">
+      <c r="H201" s="5">
         <v>19127.7117</v>
       </c>
-      <c r="I201" s="7">
+      <c r="I201" s="5">
         <v>18563.495800000001</v>
       </c>
-      <c r="J201" s="7">
+      <c r="J201" s="5">
         <v>19067.151900000001</v>
       </c>
-      <c r="K201" s="7">
+      <c r="K201" s="5">
         <v>19439.058099999998</v>
       </c>
-      <c r="L201" s="7">
+      <c r="L201" s="5">
         <v>19807.09</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12">
+      <c r="A202" s="4">
+        <v>2018</v>
+      </c>
+      <c r="B202" s="4">
+        <v>4</v>
+      </c>
+      <c r="C202" s="5">
+        <v>18671.5</v>
+      </c>
+      <c r="D202" s="5">
+        <v>18792.340800000002</v>
+      </c>
+      <c r="E202" s="5">
+        <v>18905.305199999999</v>
+      </c>
+      <c r="F202" s="5">
+        <v>19025.6453</v>
+      </c>
+      <c r="G202" s="5">
+        <v>19137.867200000001</v>
+      </c>
+      <c r="H202" s="5">
+        <v>19243.9797</v>
+      </c>
+      <c r="I202" s="5">
+        <v>18575.6993</v>
+      </c>
+      <c r="J202" s="5">
+        <v>19080.488600000001</v>
+      </c>
+      <c r="K202" s="5">
+        <v>19463.542799999999</v>
+      </c>
+      <c r="L202" s="5">
+        <v>19860.466100000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>